<commit_message>
Fichier Excel Date Horaire
</commit_message>
<xml_diff>
--- a/HORAIRE/ANNÉE 2018/template new horare.xlsx
+++ b/HORAIRE/ANNÉE 2018/template new horare.xlsx
@@ -119,11 +119,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="165" formatCode="mm"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,12 +176,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -536,7 +529,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -589,7 +582,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -629,6 +621,87 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -647,15 +720,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -665,82 +729,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -748,6 +737,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -756,6 +748,28 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/activeX/activeX1.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{20DD1B9E-87C4-11D1-8BE3-0000F8754DA1}" ax:license="651A8940-87C5-11d1-8BE3-0000F8754DA1" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="_ExtentX" ax:value="1905"/>
+  <ax:ocxPr ax:name="_ExtentY" ax:value="1905"/>
+  <ax:ocxPr ax:name="_Version" ax:value="393216"/>
+  <ax:ocxPr ax:name="Font">
+    <ax:font ax:persistence="persistPropertyBag">
+      <ax:ocxPr ax:name="Name" ax:value="Britannic Bold"/>
+      <ax:ocxPr ax:name="Size" ax:value="18"/>
+      <ax:ocxPr ax:name="Charset" ax:value="0"/>
+      <ax:ocxPr ax:name="Weight" ax:value="400"/>
+      <ax:ocxPr ax:name="Underline" ax:value="0"/>
+      <ax:ocxPr ax:name="Italic" ax:value="0"/>
+      <ax:ocxPr ax:name="Strikethrough" ax:value="0"/>
+    </ax:font>
+  </ax:ocxPr>
+  <ax:ocxPr ax:name="DateIsNull" ax:value="1"/>
+  <ax:ocxPr ax:name="Format" ax:value="662831105"/>
+  <ax:ocxPr ax:name="CurrentDate" ax:value="43610"/>
+</ax:ocx>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1046,10 +1060,10 @@
   <sheetPr codeName="Feuil1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B3:O40"/>
+  <dimension ref="B3:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="55" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="C1" zoomScale="85" zoomScaleNormal="55" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1062,40 +1076,40 @@
     <col min="13" max="13" width="2.7109375" style="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:15" ht="46.5">
-      <c r="C3" s="60" t="s">
+    <row r="3" spans="2:14" ht="46.5">
+      <c r="C3" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
-      <c r="K3" s="60"/>
-      <c r="L3" s="60"/>
-    </row>
-    <row r="4" spans="2:15" ht="22.5" customHeight="1">
-      <c r="C4" s="61" t="str">
-        <f>D6&amp;" MAI AU "&amp;J6&amp;" MAI"</f>
-        <v>20 MAI AU 26 MAI</v>
-      </c>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
-      <c r="H4" s="61"/>
-      <c r="I4" s="61"/>
-      <c r="J4" s="61"/>
-      <c r="K4" s="61"/>
-      <c r="L4" s="61"/>
-    </row>
-    <row r="5" spans="2:15" ht="36" customHeight="1">
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+    </row>
+    <row r="4" spans="2:14" ht="22.5" customHeight="1">
+      <c r="C4" s="34" t="str">
+        <f>DAY(N3)&amp;" MAI AU "&amp;J6&amp;" MAI"</f>
+        <v>0 MAI AU 26 MAI</v>
+      </c>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="34"/>
+    </row>
+    <row r="5" spans="2:14" ht="36" customHeight="1">
       <c r="E5" s="1"/>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="2:15" ht="22.5" customHeight="1" thickBot="1">
+    <row r="6" spans="2:14" ht="22.5" customHeight="1" thickBot="1">
       <c r="D6" s="3">
         <v>20</v>
       </c>
@@ -1117,12 +1131,9 @@
       <c r="J6" s="3">
         <v>26</v>
       </c>
-      <c r="O6">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="7" spans="2:15" ht="20.100000000000001" customHeight="1">
-      <c r="B7" s="50" t="s">
+    </row>
+    <row r="7" spans="2:14" ht="20.100000000000001" customHeight="1">
+      <c r="B7" s="53" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="5"/>
@@ -1147,228 +1158,225 @@
       <c r="J7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="K7" s="67" t="s">
-        <v>8</v>
-      </c>
-      <c r="L7" s="68"/>
-    </row>
-    <row r="8" spans="2:15" ht="20.100000000000001" customHeight="1">
-      <c r="B8" s="50"/>
-      <c r="C8" s="51" t="s">
+      <c r="K7" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="L7" s="44"/>
+    </row>
+    <row r="8" spans="2:14" ht="20.100000000000001" customHeight="1">
+      <c r="B8" s="53"/>
+      <c r="C8" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="30" t="s">
+      <c r="D8" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="30" t="s">
+      <c r="E8" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="30" t="s">
+      <c r="F8" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="30" t="s">
+      <c r="G8" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="30" t="s">
+      <c r="H8" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="29"/>
-      <c r="J8" s="29"/>
-      <c r="K8" s="53">
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="48">
         <f>SUM(D9+E9+F9+G9+H9+I9+J9)</f>
         <v>40</v>
       </c>
-      <c r="L8" s="65" t="s">
+      <c r="L8" s="41" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="2:15" ht="19.5" customHeight="1">
-      <c r="B9" s="50"/>
-      <c r="C9" s="52"/>
-      <c r="D9" s="28">
-        <v>8</v>
-      </c>
-      <c r="E9" s="28">
-        <v>8</v>
-      </c>
-      <c r="F9" s="28">
-        <v>8</v>
-      </c>
-      <c r="G9" s="28">
-        <v>8</v>
-      </c>
-      <c r="H9" s="28">
-        <v>8</v>
-      </c>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="54"/>
-      <c r="L9" s="69"/>
-      <c r="O9" s="20">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="2:15" ht="20.100000000000001" customHeight="1">
-      <c r="B10" s="50"/>
-      <c r="C10" s="40" t="s">
+    <row r="9" spans="2:14" ht="19.5" customHeight="1">
+      <c r="B9" s="53"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="27">
+        <v>8</v>
+      </c>
+      <c r="E9" s="27">
+        <v>8</v>
+      </c>
+      <c r="F9" s="27">
+        <v>8</v>
+      </c>
+      <c r="G9" s="27">
+        <v>8</v>
+      </c>
+      <c r="H9" s="27">
+        <v>8</v>
+      </c>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="49"/>
+      <c r="L9" s="45"/>
+    </row>
+    <row r="10" spans="2:14" ht="20.100000000000001" customHeight="1">
+      <c r="B10" s="53"/>
+      <c r="C10" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="31" t="s">
+      <c r="D10" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="31" t="s">
+      <c r="E10" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="31" t="s">
+      <c r="F10" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="31" t="s">
+      <c r="G10" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="H10" s="31" t="s">
+      <c r="H10" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="I10" s="23"/>
-      <c r="J10" s="23"/>
-      <c r="K10" s="53">
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="48">
         <f t="shared" ref="K10" si="0">SUM(D11+E11+F11+G11+H11+I11+J11)</f>
         <v>40</v>
       </c>
-      <c r="L10" s="55" t="s">
+      <c r="L10" s="46" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="2:15" ht="20.100000000000001" customHeight="1">
-      <c r="B11" s="50"/>
-      <c r="C11" s="58"/>
-      <c r="D11" s="26">
-        <v>8</v>
-      </c>
-      <c r="E11" s="26">
-        <v>8</v>
-      </c>
-      <c r="F11" s="26">
-        <v>8</v>
-      </c>
-      <c r="G11" s="26">
-        <v>8</v>
-      </c>
-      <c r="H11" s="26">
-        <v>8</v>
-      </c>
-      <c r="I11" s="27"/>
-      <c r="J11" s="27"/>
-      <c r="K11" s="54"/>
-      <c r="L11" s="59"/>
-    </row>
-    <row r="12" spans="2:15" ht="20.100000000000001" customHeight="1">
-      <c r="B12" s="50"/>
-      <c r="C12" s="40" t="s">
+    <row r="11" spans="2:14" ht="20.100000000000001" customHeight="1">
+      <c r="B11" s="53"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="25">
+        <v>8</v>
+      </c>
+      <c r="E11" s="25">
+        <v>8</v>
+      </c>
+      <c r="F11" s="25">
+        <v>8</v>
+      </c>
+      <c r="G11" s="25">
+        <v>8</v>
+      </c>
+      <c r="H11" s="25">
+        <v>8</v>
+      </c>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="49"/>
+      <c r="L11" s="47"/>
+    </row>
+    <row r="12" spans="2:14" ht="20.100000000000001" customHeight="1">
+      <c r="B12" s="53"/>
+      <c r="C12" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33" t="s">
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="G12" s="33" t="s">
+      <c r="G12" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="H12" s="33" t="s">
+      <c r="H12" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="I12" s="33" t="s">
+      <c r="I12" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="J12" s="24" t="s">
+      <c r="J12" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="K12" s="53">
+      <c r="K12" s="48">
         <f t="shared" ref="K12" si="1">SUM(D13+E13+F13+G13+H13+I13+J13)</f>
         <v>30</v>
       </c>
-      <c r="L12" s="55" t="s">
+      <c r="L12" s="46" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="2:15" ht="20.100000000000001" customHeight="1">
-      <c r="B13" s="50"/>
-      <c r="C13" s="58"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27">
+    <row r="13" spans="2:14" ht="20.100000000000001" customHeight="1">
+      <c r="B13" s="53"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26">
         <v>6</v>
       </c>
-      <c r="G13" s="27">
+      <c r="G13" s="26">
         <v>6</v>
       </c>
-      <c r="H13" s="27">
+      <c r="H13" s="26">
         <v>6</v>
       </c>
-      <c r="I13" s="27">
+      <c r="I13" s="26">
         <v>6</v>
       </c>
-      <c r="J13" s="27">
+      <c r="J13" s="26">
         <v>6</v>
       </c>
-      <c r="K13" s="54"/>
-      <c r="L13" s="55"/>
+      <c r="K13" s="49"/>
+      <c r="L13" s="46"/>
       <c r="N13" s="8"/>
     </row>
-    <row r="14" spans="2:15" ht="20.100000000000001" customHeight="1">
-      <c r="B14" s="50"/>
-      <c r="C14" s="40" t="s">
+    <row r="14" spans="2:14" ht="20.100000000000001" customHeight="1">
+      <c r="B14" s="53"/>
+      <c r="C14" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="24" t="s">
+      <c r="D14" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24" t="s">
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="H14" s="24" t="s">
+      <c r="H14" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="I14" s="24" t="s">
+      <c r="I14" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="J14" s="24" t="s">
+      <c r="J14" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="K14" s="53">
+      <c r="K14" s="48">
         <f t="shared" ref="K14" si="2">SUM(D15+E15+F15+G15+H15+I15+J15)</f>
         <v>34</v>
       </c>
-      <c r="L14" s="65" t="s">
+      <c r="L14" s="41" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="2:15" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B15" s="50"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="27">
+    <row r="15" spans="2:14" ht="20.100000000000001" customHeight="1" thickBot="1">
+      <c r="B15" s="53"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="26">
         <v>6</v>
       </c>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27">
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26">
         <v>6</v>
       </c>
-      <c r="H15" s="27">
+      <c r="H15" s="26">
         <v>6</v>
       </c>
-      <c r="I15" s="27">
-        <v>8</v>
-      </c>
-      <c r="J15" s="27">
-        <v>8</v>
-      </c>
-      <c r="K15" s="70"/>
-      <c r="L15" s="66"/>
-    </row>
-    <row r="16" spans="2:15" ht="47.25" customHeight="1" thickBot="1">
+      <c r="I15" s="26">
+        <v>8</v>
+      </c>
+      <c r="J15" s="26">
+        <v>8</v>
+      </c>
+      <c r="K15" s="52"/>
+      <c r="L15" s="42"/>
+    </row>
+    <row r="16" spans="2:14" ht="47.25" customHeight="1" thickBot="1">
       <c r="B16" s="15"/>
     </row>
     <row r="17" spans="2:12" ht="20.100000000000001" customHeight="1">
@@ -1397,122 +1405,122 @@
       <c r="J17" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="K17" s="67" t="s">
-        <v>8</v>
-      </c>
-      <c r="L17" s="68"/>
+      <c r="K17" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="L17" s="44"/>
     </row>
     <row r="18" spans="2:12" ht="20.100000000000001" customHeight="1">
       <c r="B18" s="56"/>
-      <c r="C18" s="51" t="s">
+      <c r="C18" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="21"/>
-      <c r="J18" s="21"/>
-      <c r="K18" s="42"/>
-      <c r="L18" s="65"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="57"/>
+      <c r="L18" s="41"/>
     </row>
     <row r="19" spans="2:12" ht="20.100000000000001" customHeight="1">
       <c r="B19" s="56"/>
-      <c r="C19" s="52"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="25"/>
-      <c r="J19" s="25"/>
-      <c r="K19" s="57"/>
-      <c r="L19" s="69"/>
+      <c r="C19" s="55"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="58"/>
+      <c r="L19" s="45"/>
     </row>
     <row r="20" spans="2:12" ht="20.100000000000001" customHeight="1">
       <c r="B20" s="56"/>
-      <c r="C20" s="40" t="s">
+      <c r="C20" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="22"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="23"/>
-      <c r="J20" s="23"/>
-      <c r="K20" s="42"/>
-      <c r="L20" s="55"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
+      <c r="K20" s="57"/>
+      <c r="L20" s="46"/>
     </row>
     <row r="21" spans="2:12" ht="20.100000000000001" customHeight="1">
       <c r="B21" s="56"/>
-      <c r="C21" s="58"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="27"/>
-      <c r="I21" s="27"/>
-      <c r="J21" s="27"/>
-      <c r="K21" s="57"/>
-      <c r="L21" s="59"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="58"/>
+      <c r="L21" s="47"/>
     </row>
     <row r="22" spans="2:12" ht="20.100000000000001" customHeight="1">
       <c r="B22" s="56"/>
-      <c r="C22" s="40" t="s">
+      <c r="C22" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
-      <c r="I22" s="24"/>
-      <c r="J22" s="24"/>
-      <c r="K22" s="42"/>
-      <c r="L22" s="55"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="57"/>
+      <c r="L22" s="46"/>
     </row>
     <row r="23" spans="2:12" ht="20.100000000000001" customHeight="1">
       <c r="B23" s="56"/>
-      <c r="C23" s="58"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="27"/>
-      <c r="I23" s="27"/>
-      <c r="J23" s="27"/>
-      <c r="K23" s="57"/>
-      <c r="L23" s="55"/>
+      <c r="C23" s="59"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="58"/>
+      <c r="L23" s="46"/>
     </row>
     <row r="24" spans="2:12" ht="20.100000000000001" customHeight="1">
       <c r="B24" s="56"/>
-      <c r="C24" s="40" t="s">
+      <c r="C24" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="24"/>
-      <c r="I24" s="24"/>
-      <c r="J24" s="24"/>
-      <c r="K24" s="42"/>
-      <c r="L24" s="65"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="23"/>
+      <c r="K24" s="57"/>
+      <c r="L24" s="41"/>
     </row>
     <row r="25" spans="2:12" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="B25" s="56"/>
-      <c r="C25" s="41"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="27"/>
-      <c r="I25" s="27"/>
-      <c r="J25" s="27"/>
-      <c r="K25" s="43"/>
-      <c r="L25" s="66"/>
+      <c r="C25" s="51"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="26"/>
+      <c r="K25" s="66"/>
+      <c r="L25" s="42"/>
     </row>
     <row r="30" spans="2:12">
       <c r="E30" s="9" t="s">
@@ -1532,7 +1540,7 @@
       </c>
     </row>
     <row r="31" spans="2:12">
-      <c r="E31" s="62" t="s">
+      <c r="E31" s="35" t="s">
         <v>9</v>
       </c>
       <c r="F31" s="10" t="s">
@@ -1542,16 +1550,16 @@
         <f>K8</f>
         <v>40</v>
       </c>
-      <c r="H31" s="46">
+      <c r="H31" s="37">
         <f>G32-G31</f>
         <v>-40</v>
       </c>
-      <c r="I31" s="64">
+      <c r="I31" s="39">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="2:12">
-      <c r="E32" s="63"/>
+      <c r="E32" s="36"/>
       <c r="F32" s="11" t="s">
         <v>17</v>
       </c>
@@ -1559,11 +1567,11 @@
         <f>K9</f>
         <v>0</v>
       </c>
-      <c r="H32" s="47"/>
-      <c r="I32" s="48"/>
+      <c r="H32" s="38"/>
+      <c r="I32" s="40"/>
     </row>
     <row r="33" spans="5:9">
-      <c r="E33" s="44" t="s">
+      <c r="E33" s="67" t="s">
         <v>10</v>
       </c>
       <c r="F33" s="11" t="s">
@@ -1573,17 +1581,17 @@
         <f>K10</f>
         <v>40</v>
       </c>
-      <c r="H33" s="46">
+      <c r="H33" s="37">
         <f>G34-G33</f>
         <v>-40</v>
       </c>
-      <c r="I33" s="48">
+      <c r="I33" s="40">
         <f>G34/G33</f>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="5:9">
-      <c r="E34" s="49"/>
+      <c r="E34" s="69"/>
       <c r="F34" s="11" t="s">
         <v>17</v>
       </c>
@@ -1591,11 +1599,11 @@
         <f>K20</f>
         <v>0</v>
       </c>
-      <c r="H34" s="47"/>
-      <c r="I34" s="48"/>
+      <c r="H34" s="38"/>
+      <c r="I34" s="40"/>
     </row>
     <row r="35" spans="5:9">
-      <c r="E35" s="44" t="s">
+      <c r="E35" s="67" t="s">
         <v>11</v>
       </c>
       <c r="F35" s="11" t="s">
@@ -1605,17 +1613,17 @@
         <f>K12</f>
         <v>30</v>
       </c>
-      <c r="H35" s="46">
+      <c r="H35" s="37">
         <f>G36-G35</f>
         <v>-30</v>
       </c>
-      <c r="I35" s="48">
+      <c r="I35" s="40">
         <f>G36/G35</f>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="5:9">
-      <c r="E36" s="49"/>
+      <c r="E36" s="69"/>
       <c r="F36" s="11" t="s">
         <v>17</v>
       </c>
@@ -1623,11 +1631,11 @@
         <f>K22</f>
         <v>0</v>
       </c>
-      <c r="H36" s="47"/>
-      <c r="I36" s="48"/>
+      <c r="H36" s="38"/>
+      <c r="I36" s="40"/>
     </row>
     <row r="37" spans="5:9">
-      <c r="E37" s="44" t="s">
+      <c r="E37" s="67" t="s">
         <v>12</v>
       </c>
       <c r="F37" s="11" t="s">
@@ -1637,17 +1645,17 @@
         <f>K14</f>
         <v>34</v>
       </c>
-      <c r="H37" s="46">
+      <c r="H37" s="37">
         <f>G38-G37</f>
         <v>-34</v>
       </c>
-      <c r="I37" s="48">
+      <c r="I37" s="40">
         <f>G38/G37</f>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="5:9" ht="15.75" thickBot="1">
-      <c r="E38" s="45"/>
+      <c r="E38" s="68"/>
       <c r="F38" s="11" t="s">
         <v>17</v>
       </c>
@@ -1655,11 +1663,11 @@
         <f>K24</f>
         <v>0</v>
       </c>
-      <c r="H38" s="47"/>
-      <c r="I38" s="48"/>
+      <c r="H38" s="38"/>
+      <c r="I38" s="40"/>
     </row>
     <row r="39" spans="5:9">
-      <c r="E39" s="38" t="s">
+      <c r="E39" s="64" t="s">
         <v>8</v>
       </c>
       <c r="F39" s="16" t="s">
@@ -1669,17 +1677,17 @@
         <f>SUM(K8+K10+K12+K14)</f>
         <v>144</v>
       </c>
-      <c r="H39" s="34">
+      <c r="H39" s="60">
         <f>G40-G39</f>
         <v>-144</v>
       </c>
-      <c r="I39" s="36">
+      <c r="I39" s="62">
         <f>G40/G39</f>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="5:9" ht="15.75" thickBot="1">
-      <c r="E40" s="39"/>
+      <c r="E40" s="65"/>
       <c r="F40" s="17" t="s">
         <v>23</v>
       </c>
@@ -1687,11 +1695,40 @@
         <f>K18+K20+K22+K24</f>
         <v>0</v>
       </c>
-      <c r="H40" s="35"/>
-      <c r="I40" s="37"/>
+      <c r="H40" s="61"/>
+      <c r="I40" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="45">
+    <mergeCell ref="H39:H40"/>
+    <mergeCell ref="I39:I40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="K24:K25"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="H37:H38"/>
+    <mergeCell ref="I37:I38"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="H33:H34"/>
+    <mergeCell ref="I33:I34"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="H35:H36"/>
+    <mergeCell ref="I35:I36"/>
+    <mergeCell ref="B7:B15"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="B17:B25"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="K20:K21"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="L20:L21"/>
     <mergeCell ref="C3:L3"/>
     <mergeCell ref="C4:L4"/>
     <mergeCell ref="E31:E32"/>
@@ -1708,39 +1745,14 @@
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="K14:K15"/>
     <mergeCell ref="L18:L19"/>
-    <mergeCell ref="B7:B15"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="B17:B25"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="K20:K21"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="L20:L21"/>
-    <mergeCell ref="H39:H40"/>
-    <mergeCell ref="I39:I40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="K24:K25"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="H37:H38"/>
-    <mergeCell ref="I37:I38"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="H33:H34"/>
-    <mergeCell ref="I33:I34"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="H35:H36"/>
-    <mergeCell ref="I35:I36"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.71212121212121215" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup scale="65" orientation="landscape" horizontalDpi="4294967294" verticalDpi="4294967294" r:id="rId1"/>
+  <pageSetup scale="61" orientation="landscape" horizontalDpi="4294967294" verticalDpi="4294967294" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <controls>
+    <control shapeId="1026" r:id="rId3" name="DTPicker1"/>
+  </controls>
 </worksheet>
 </file>
 
@@ -1765,33 +1777,33 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:14" ht="46.5">
-      <c r="C3" s="60" t="s">
+      <c r="C3" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
-      <c r="K3" s="60"/>
-      <c r="L3" s="60"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
     </row>
     <row r="4" spans="2:14" ht="22.5" customHeight="1">
-      <c r="C4" s="61" t="str">
+      <c r="C4" s="34" t="str">
         <f>D6&amp;" AVRIL AU "&amp;J6&amp;" JUIN"</f>
         <v>27 AVRIL AU 2 JUIN</v>
       </c>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
-      <c r="H4" s="61"/>
-      <c r="I4" s="61"/>
-      <c r="J4" s="61"/>
-      <c r="K4" s="61"/>
-      <c r="L4" s="61"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="34"/>
     </row>
     <row r="5" spans="2:14" ht="36" customHeight="1">
       <c r="E5" s="1"/>
@@ -1822,248 +1834,248 @@
       </c>
     </row>
     <row r="7" spans="2:14" ht="20.100000000000001" customHeight="1">
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="53" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="5"/>
-      <c r="D7" s="32" t="s">
+      <c r="D7" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="32" t="s">
+      <c r="E7" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="32" t="s">
+      <c r="F7" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="32" t="s">
+      <c r="G7" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="32" t="s">
+      <c r="H7" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="32" t="s">
+      <c r="I7" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="32" t="s">
+      <c r="J7" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="K7" s="71" t="s">
-        <v>8</v>
-      </c>
-      <c r="L7" s="68"/>
+      <c r="K7" s="72" t="s">
+        <v>8</v>
+      </c>
+      <c r="L7" s="44"/>
     </row>
     <row r="8" spans="2:14" ht="20.100000000000001" customHeight="1">
-      <c r="B8" s="50"/>
-      <c r="C8" s="51" t="s">
+      <c r="B8" s="53"/>
+      <c r="C8" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="30" t="s">
+      <c r="D8" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="30" t="s">
+      <c r="E8" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="30" t="s">
+      <c r="F8" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="30" t="s">
+      <c r="G8" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="30" t="s">
+      <c r="H8" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="29"/>
-      <c r="J8" s="29"/>
-      <c r="K8" s="53">
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="48">
         <f>SUM(D9+E9+F9+G9+H9+I9+J9)</f>
         <v>40</v>
       </c>
-      <c r="L8" s="65" t="s">
+      <c r="L8" s="41" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="2:14" ht="20.100000000000001" customHeight="1">
-      <c r="B9" s="50"/>
-      <c r="C9" s="52"/>
-      <c r="D9" s="28">
-        <v>8</v>
-      </c>
-      <c r="E9" s="28">
-        <v>8</v>
-      </c>
-      <c r="F9" s="28">
-        <v>8</v>
-      </c>
-      <c r="G9" s="28">
-        <v>8</v>
-      </c>
-      <c r="H9" s="28">
-        <v>8</v>
-      </c>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="54"/>
-      <c r="L9" s="69"/>
+      <c r="B9" s="53"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="27">
+        <v>8</v>
+      </c>
+      <c r="E9" s="27">
+        <v>8</v>
+      </c>
+      <c r="F9" s="27">
+        <v>8</v>
+      </c>
+      <c r="G9" s="27">
+        <v>8</v>
+      </c>
+      <c r="H9" s="27">
+        <v>8</v>
+      </c>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="49"/>
+      <c r="L9" s="45"/>
     </row>
     <row r="10" spans="2:14" ht="20.100000000000001" customHeight="1">
-      <c r="B10" s="50"/>
-      <c r="C10" s="40" t="s">
+      <c r="B10" s="53"/>
+      <c r="C10" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="31" t="s">
+      <c r="D10" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="31" t="s">
+      <c r="E10" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="31" t="s">
+      <c r="F10" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="31" t="s">
+      <c r="G10" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="H10" s="31" t="s">
+      <c r="H10" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="I10" s="23"/>
-      <c r="J10" s="23"/>
-      <c r="K10" s="42">
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="57">
         <f t="shared" ref="K10" si="0">SUM(D11+E11+F11+G11+H11+I11+J11)</f>
         <v>40</v>
       </c>
-      <c r="L10" s="55" t="s">
+      <c r="L10" s="46" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="11" spans="2:14" ht="20.100000000000001" customHeight="1">
-      <c r="B11" s="50"/>
-      <c r="C11" s="58"/>
-      <c r="D11" s="26">
-        <v>8</v>
-      </c>
-      <c r="E11" s="26">
-        <v>8</v>
-      </c>
-      <c r="F11" s="26">
-        <v>8</v>
-      </c>
-      <c r="G11" s="26">
-        <v>8</v>
-      </c>
-      <c r="H11" s="26">
-        <v>8</v>
-      </c>
-      <c r="I11" s="27"/>
-      <c r="J11" s="27"/>
-      <c r="K11" s="57"/>
-      <c r="L11" s="59"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="25">
+        <v>8</v>
+      </c>
+      <c r="E11" s="25">
+        <v>8</v>
+      </c>
+      <c r="F11" s="25">
+        <v>8</v>
+      </c>
+      <c r="G11" s="25">
+        <v>8</v>
+      </c>
+      <c r="H11" s="25">
+        <v>8</v>
+      </c>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="58"/>
+      <c r="L11" s="47"/>
     </row>
     <row r="12" spans="2:14" ht="20.100000000000001" customHeight="1">
-      <c r="B12" s="50"/>
-      <c r="C12" s="40" t="s">
+      <c r="B12" s="53"/>
+      <c r="C12" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33" t="s">
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="G12" s="33" t="s">
+      <c r="G12" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="H12" s="33" t="s">
+      <c r="H12" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="I12" s="33" t="s">
+      <c r="I12" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="J12" s="24" t="s">
+      <c r="J12" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="K12" s="42">
+      <c r="K12" s="57">
         <f t="shared" ref="K12" si="1">SUM(D13+E13+F13+G13+H13+I13+J13)</f>
         <v>30</v>
       </c>
-      <c r="L12" s="55" t="s">
+      <c r="L12" s="46" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="13" spans="2:14" ht="20.100000000000001" customHeight="1">
-      <c r="B13" s="50"/>
-      <c r="C13" s="58"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27">
+      <c r="B13" s="53"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26">
         <v>6</v>
       </c>
-      <c r="G13" s="27">
+      <c r="G13" s="26">
         <v>6</v>
       </c>
-      <c r="H13" s="27">
+      <c r="H13" s="26">
         <v>6</v>
       </c>
-      <c r="I13" s="27">
+      <c r="I13" s="26">
         <v>6</v>
       </c>
-      <c r="J13" s="27">
+      <c r="J13" s="26">
         <v>6</v>
       </c>
-      <c r="K13" s="57"/>
-      <c r="L13" s="55"/>
+      <c r="K13" s="58"/>
+      <c r="L13" s="46"/>
       <c r="N13" s="8"/>
     </row>
     <row r="14" spans="2:14" ht="20.100000000000001" customHeight="1">
-      <c r="B14" s="50"/>
-      <c r="C14" s="40" t="s">
+      <c r="B14" s="53"/>
+      <c r="C14" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="24" t="s">
+      <c r="D14" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24" t="s">
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="H14" s="24" t="s">
+      <c r="H14" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="I14" s="24" t="s">
+      <c r="I14" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="J14" s="24" t="s">
+      <c r="J14" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="K14" s="42">
+      <c r="K14" s="57">
         <f>SUM(D15+E15+F15+G15+H15+I15+J15)</f>
         <v>34</v>
       </c>
-      <c r="L14" s="65" t="s">
+      <c r="L14" s="41" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="15" spans="2:14" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B15" s="50"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="27">
+      <c r="B15" s="53"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="26">
         <v>6</v>
       </c>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27">
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26">
         <v>6</v>
       </c>
-      <c r="H15" s="27">
+      <c r="H15" s="26">
         <v>6</v>
       </c>
-      <c r="I15" s="27">
-        <v>8</v>
-      </c>
-      <c r="J15" s="27">
-        <v>8</v>
-      </c>
-      <c r="K15" s="43"/>
-      <c r="L15" s="66"/>
+      <c r="I15" s="26">
+        <v>8</v>
+      </c>
+      <c r="J15" s="26">
+        <v>8</v>
+      </c>
+      <c r="K15" s="66"/>
+      <c r="L15" s="42"/>
     </row>
     <row r="16" spans="2:14" ht="47.25" customHeight="1" thickBot="1">
       <c r="B16" s="15"/>
@@ -2094,142 +2106,142 @@
       <c r="J17" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="K17" s="67" t="s">
-        <v>8</v>
-      </c>
-      <c r="L17" s="68"/>
+      <c r="K17" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="L17" s="44"/>
     </row>
     <row r="18" spans="2:12" ht="20.100000000000001" customHeight="1">
       <c r="B18" s="56"/>
-      <c r="C18" s="51" t="s">
+      <c r="C18" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="21"/>
-      <c r="J18" s="21"/>
-      <c r="K18" s="42">
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="57">
         <f>SUM(D19+E19+F19+G19+H19+I19+J19)</f>
         <v>0</v>
       </c>
-      <c r="L18" s="65" t="s">
+      <c r="L18" s="41" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="19" spans="2:12" ht="20.100000000000001" customHeight="1">
       <c r="B19" s="56"/>
-      <c r="C19" s="52"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="25"/>
-      <c r="J19" s="25"/>
-      <c r="K19" s="57"/>
-      <c r="L19" s="69"/>
+      <c r="C19" s="55"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="58"/>
+      <c r="L19" s="45"/>
     </row>
     <row r="20" spans="2:12" ht="20.100000000000001" customHeight="1">
       <c r="B20" s="56"/>
-      <c r="C20" s="40" t="s">
+      <c r="C20" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="22"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="23"/>
-      <c r="J20" s="23"/>
-      <c r="K20" s="42">
+      <c r="D20" s="21"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
+      <c r="K20" s="57">
         <f>SUM(D21+E21+F21+G21+H21+I21+J21)</f>
         <v>0</v>
       </c>
-      <c r="L20" s="55" t="s">
+      <c r="L20" s="46" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="21" spans="2:12" ht="20.100000000000001" customHeight="1">
       <c r="B21" s="56"/>
-      <c r="C21" s="58"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="27"/>
-      <c r="I21" s="27"/>
-      <c r="J21" s="27"/>
-      <c r="K21" s="57"/>
-      <c r="L21" s="59"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="58"/>
+      <c r="L21" s="47"/>
     </row>
     <row r="22" spans="2:12" ht="20.100000000000001" customHeight="1">
       <c r="B22" s="56"/>
-      <c r="C22" s="40" t="s">
+      <c r="C22" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
-      <c r="I22" s="24"/>
-      <c r="J22" s="24"/>
-      <c r="K22" s="42">
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="57">
         <f t="shared" ref="K22" si="2">SUM(D23+E23+F23+G23+H23+I23+J23)</f>
         <v>0</v>
       </c>
-      <c r="L22" s="55" t="s">
+      <c r="L22" s="46" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="23" spans="2:12" ht="20.100000000000001" customHeight="1">
       <c r="B23" s="56"/>
-      <c r="C23" s="58"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="27"/>
-      <c r="I23" s="27"/>
-      <c r="J23" s="27"/>
-      <c r="K23" s="57"/>
-      <c r="L23" s="55"/>
+      <c r="C23" s="59"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="58"/>
+      <c r="L23" s="46"/>
     </row>
     <row r="24" spans="2:12" ht="20.100000000000001" customHeight="1">
       <c r="B24" s="56"/>
-      <c r="C24" s="40" t="s">
+      <c r="C24" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="24"/>
-      <c r="I24" s="24"/>
-      <c r="J24" s="24"/>
-      <c r="K24" s="42">
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="23"/>
+      <c r="K24" s="57">
         <f t="shared" ref="K24" si="3">SUM(D25+E25+F25+G25+H25+I25+J25)</f>
         <v>0</v>
       </c>
-      <c r="L24" s="65" t="s">
+      <c r="L24" s="41" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="25" spans="2:12" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="B25" s="56"/>
-      <c r="C25" s="41"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="27"/>
-      <c r="I25" s="27"/>
-      <c r="J25" s="27"/>
-      <c r="K25" s="43"/>
-      <c r="L25" s="66"/>
+      <c r="C25" s="51"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="26"/>
+      <c r="K25" s="66"/>
+      <c r="L25" s="42"/>
     </row>
     <row r="30" spans="2:12">
       <c r="E30" s="9" t="s">
@@ -2249,7 +2261,7 @@
       </c>
     </row>
     <row r="31" spans="2:12">
-      <c r="E31" s="62" t="s">
+      <c r="E31" s="35" t="s">
         <v>9</v>
       </c>
       <c r="F31" s="10" t="s">
@@ -2259,16 +2271,16 @@
         <f>K8</f>
         <v>40</v>
       </c>
-      <c r="H31" s="46">
+      <c r="H31" s="37">
         <f>G32-G31</f>
         <v>-40</v>
       </c>
-      <c r="I31" s="64">
+      <c r="I31" s="39">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="2:12">
-      <c r="E32" s="63"/>
+      <c r="E32" s="36"/>
       <c r="F32" s="11" t="s">
         <v>17</v>
       </c>
@@ -2276,11 +2288,11 @@
         <f>K18</f>
         <v>0</v>
       </c>
-      <c r="H32" s="47"/>
-      <c r="I32" s="48"/>
+      <c r="H32" s="38"/>
+      <c r="I32" s="40"/>
     </row>
     <row r="33" spans="5:9">
-      <c r="E33" s="44" t="s">
+      <c r="E33" s="67" t="s">
         <v>10</v>
       </c>
       <c r="F33" s="11" t="s">
@@ -2290,17 +2302,17 @@
         <f>K10</f>
         <v>40</v>
       </c>
-      <c r="H33" s="46">
+      <c r="H33" s="37">
         <f>G34-G33</f>
         <v>-40</v>
       </c>
-      <c r="I33" s="48">
+      <c r="I33" s="40">
         <f>G34/G33</f>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="5:9">
-      <c r="E34" s="49"/>
+      <c r="E34" s="69"/>
       <c r="F34" s="11" t="s">
         <v>17</v>
       </c>
@@ -2308,11 +2320,11 @@
         <f>K20</f>
         <v>0</v>
       </c>
-      <c r="H34" s="47"/>
-      <c r="I34" s="48"/>
+      <c r="H34" s="38"/>
+      <c r="I34" s="40"/>
     </row>
     <row r="35" spans="5:9">
-      <c r="E35" s="44" t="s">
+      <c r="E35" s="67" t="s">
         <v>11</v>
       </c>
       <c r="F35" s="11" t="s">
@@ -2322,17 +2334,17 @@
         <f>K12</f>
         <v>30</v>
       </c>
-      <c r="H35" s="46">
+      <c r="H35" s="37">
         <f>G36-G35</f>
         <v>-30</v>
       </c>
-      <c r="I35" s="48">
+      <c r="I35" s="40">
         <f>G36/G35</f>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="5:9">
-      <c r="E36" s="49"/>
+      <c r="E36" s="69"/>
       <c r="F36" s="11" t="s">
         <v>17</v>
       </c>
@@ -2340,11 +2352,11 @@
         <f>K22</f>
         <v>0</v>
       </c>
-      <c r="H36" s="47"/>
-      <c r="I36" s="48"/>
+      <c r="H36" s="38"/>
+      <c r="I36" s="40"/>
     </row>
     <row r="37" spans="5:9">
-      <c r="E37" s="44" t="s">
+      <c r="E37" s="67" t="s">
         <v>12</v>
       </c>
       <c r="F37" s="11" t="s">
@@ -2354,17 +2366,17 @@
         <f>K14</f>
         <v>34</v>
       </c>
-      <c r="H37" s="46">
+      <c r="H37" s="37">
         <f>G38-G37</f>
         <v>-34</v>
       </c>
-      <c r="I37" s="48">
+      <c r="I37" s="40">
         <f>G38/G37</f>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="5:9">
-      <c r="E38" s="49"/>
+      <c r="E38" s="69"/>
       <c r="F38" s="12" t="s">
         <v>17</v>
       </c>
@@ -2372,37 +2384,11 @@
         <f>K24</f>
         <v>0</v>
       </c>
-      <c r="H38" s="72"/>
-      <c r="I38" s="73"/>
+      <c r="H38" s="70"/>
+      <c r="I38" s="71"/>
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="H31:H32"/>
-    <mergeCell ref="I31:I32"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="H37:H38"/>
-    <mergeCell ref="I37:I38"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="H33:H34"/>
-    <mergeCell ref="I33:I34"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="H35:H36"/>
-    <mergeCell ref="I35:I36"/>
-    <mergeCell ref="B17:B25"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="L18:L19"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="K20:K21"/>
-    <mergeCell ref="L20:L21"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="K24:K25"/>
-    <mergeCell ref="L24:L25"/>
     <mergeCell ref="C3:L3"/>
     <mergeCell ref="C4:L4"/>
     <mergeCell ref="B7:B15"/>
@@ -2419,6 +2405,32 @@
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="K14:K15"/>
     <mergeCell ref="L14:L15"/>
+    <mergeCell ref="B17:B25"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="L18:L19"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="K20:K21"/>
+    <mergeCell ref="L20:L21"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="K24:K25"/>
+    <mergeCell ref="L24:L25"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="I31:I32"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="H37:H38"/>
+    <mergeCell ref="I37:I38"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="H33:H34"/>
+    <mergeCell ref="I33:I34"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="H35:H36"/>
+    <mergeCell ref="I35:I36"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -2428,6 +2440,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Feuil3"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
changement chili con carne
</commit_message>
<xml_diff>
--- a/HORAIRE/ANNÉE 2018/template new horare.xlsx
+++ b/HORAIRE/ANNÉE 2018/template new horare.xlsx
@@ -4,23 +4,23 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="300" windowWidth="18495" windowHeight="11700"/>
+    <workbookView xWindow="480" yWindow="300" windowWidth="18495" windowHeight="11700" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="20-26" sheetId="2" r:id="rId1"/>
-    <sheet name="27-2" sheetId="4" r:id="rId2"/>
+    <sheet name="15-21 " sheetId="2" r:id="rId1"/>
+    <sheet name="22-28" sheetId="4" r:id="rId2"/>
     <sheet name="Feuil1" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'20-26'!$B$3:$M$25</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'27-2'!$B$3:$M$25</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'15-21 '!$B$3:$M$25</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'22-28'!$B$3:$M$25</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="32">
   <si>
     <t>HORAIRE</t>
   </si>
@@ -97,12 +97,6 @@
     <t>10H00 A 18H00</t>
   </si>
   <si>
-    <t>07H00 A 15H00</t>
-  </si>
-  <si>
-    <t>7H00 A 15H00</t>
-  </si>
-  <si>
     <t>14H00 A 20H00</t>
   </si>
   <si>
@@ -113,6 +107,15 @@
   </si>
   <si>
     <t>10H00 A 16H00</t>
+  </si>
+  <si>
+    <t>7H00 A 14H00</t>
+  </si>
+  <si>
+    <t>14H A 21H00</t>
+  </si>
+  <si>
+    <t>14H00 A 21H00</t>
   </si>
 </sst>
 </file>
@@ -122,7 +125,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,8 +179,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -202,6 +233,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="29">
     <border>
@@ -529,7 +566,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -621,6 +658,105 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -639,15 +775,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -657,82 +784,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -740,6 +792,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1062,8 +1126,8 @@
   </sheetPr>
   <dimension ref="B3:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="C1" zoomScale="85" zoomScaleNormal="55" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView view="pageLayout" topLeftCell="A3" zoomScale="85" zoomScaleNormal="55" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1077,33 +1141,33 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:14" ht="46.5">
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="59"/>
-      <c r="J3" s="59"/>
-      <c r="K3" s="59"/>
-      <c r="L3" s="59"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
     </row>
     <row r="4" spans="2:14" ht="22.5" customHeight="1">
-      <c r="C4" s="60" t="str">
-        <f>DAY(D6)&amp;" JUIN AU "&amp;J6&amp;"JUIN"</f>
-        <v>3 JUIN AU 9JUIN</v>
-      </c>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="60"/>
+      <c r="C4" s="40" t="str">
+        <f>DAY(D6)&amp;" JUILLET AU "&amp;J6&amp;"JUILLET"</f>
+        <v>15 JUILLET AU 21JUILLET</v>
+      </c>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
     </row>
     <row r="5" spans="2:14" ht="36" customHeight="1">
       <c r="E5" s="1"/>
@@ -1111,29 +1175,29 @@
     </row>
     <row r="6" spans="2:14" ht="22.5" customHeight="1" thickBot="1">
       <c r="D6" s="3">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="E6" s="4">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="F6" s="3">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="G6" s="4">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="H6" s="3">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="I6" s="4">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="J6" s="3">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="2:14" ht="20.100000000000001" customHeight="1">
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="59" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="5"/>
@@ -1158,19 +1222,17 @@
       <c r="J7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="K7" s="66" t="s">
+      <c r="K7" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="L7" s="67"/>
+      <c r="L7" s="50"/>
     </row>
     <row r="8" spans="2:14" ht="20.100000000000001" customHeight="1">
-      <c r="B8" s="49"/>
-      <c r="C8" s="50" t="s">
+      <c r="B8" s="59"/>
+      <c r="C8" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="29" t="s">
-        <v>24</v>
-      </c>
+      <c r="D8" s="29"/>
       <c r="E8" s="29" t="s">
         <v>24</v>
       </c>
@@ -1185,20 +1247,18 @@
       </c>
       <c r="I8" s="28"/>
       <c r="J8" s="28"/>
-      <c r="K8" s="52">
+      <c r="K8" s="54">
         <f>SUM(D9+E9+F9+G9+H9+I9+J9)</f>
-        <v>40</v>
-      </c>
-      <c r="L8" s="64" t="s">
+        <v>32</v>
+      </c>
+      <c r="L8" s="47" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="2:14" ht="19.5" customHeight="1">
-      <c r="B9" s="49"/>
-      <c r="C9" s="51"/>
-      <c r="D9" s="27">
-        <v>8</v>
-      </c>
+      <c r="B9" s="59"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="27"/>
       <c r="E9" s="27">
         <v>8</v>
       </c>
@@ -1213,42 +1273,42 @@
       </c>
       <c r="I9" s="24"/>
       <c r="J9" s="24"/>
-      <c r="K9" s="53"/>
-      <c r="L9" s="68"/>
+      <c r="K9" s="55"/>
+      <c r="L9" s="51"/>
     </row>
     <row r="10" spans="2:14" ht="20.100000000000001" customHeight="1">
-      <c r="B10" s="49"/>
-      <c r="C10" s="39" t="s">
+      <c r="B10" s="59"/>
+      <c r="C10" s="56" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F10" s="30" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G10" s="30" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H10" s="30" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I10" s="22"/>
       <c r="J10" s="22"/>
-      <c r="K10" s="52">
+      <c r="K10" s="54">
         <f t="shared" ref="K10" si="0">SUM(D11+E11+F11+G11+H11+I11+J11)</f>
         <v>40</v>
       </c>
-      <c r="L10" s="54" t="s">
+      <c r="L10" s="52" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="11" spans="2:14" ht="20.100000000000001" customHeight="1">
-      <c r="B11" s="49"/>
-      <c r="C11" s="57"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="65"/>
       <c r="D11" s="25">
         <v>8</v>
       </c>
@@ -1266,42 +1326,42 @@
       </c>
       <c r="I11" s="26"/>
       <c r="J11" s="26"/>
-      <c r="K11" s="53"/>
-      <c r="L11" s="58"/>
+      <c r="K11" s="55"/>
+      <c r="L11" s="53"/>
     </row>
     <row r="12" spans="2:14" ht="20.100000000000001" customHeight="1">
-      <c r="B12" s="49"/>
-      <c r="C12" s="39" t="s">
-        <v>29</v>
+      <c r="B12" s="59"/>
+      <c r="C12" s="56" t="s">
+        <v>27</v>
       </c>
       <c r="D12" s="32"/>
       <c r="E12" s="32"/>
       <c r="F12" s="32" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G12" s="32" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H12" s="32" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I12" s="32" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J12" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="K12" s="52">
+        <v>28</v>
+      </c>
+      <c r="K12" s="54">
         <f t="shared" ref="K12" si="1">SUM(D13+E13+F13+G13+H13+I13+J13)</f>
         <v>30</v>
       </c>
-      <c r="L12" s="54" t="s">
+      <c r="L12" s="52" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="13" spans="2:14" ht="20.100000000000001" customHeight="1">
-      <c r="B13" s="49"/>
-      <c r="C13" s="57"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="65"/>
       <c r="D13" s="26"/>
       <c r="E13" s="26"/>
       <c r="F13" s="26">
@@ -1319,68 +1379,62 @@
       <c r="J13" s="26">
         <v>6</v>
       </c>
-      <c r="K13" s="53"/>
-      <c r="L13" s="54"/>
+      <c r="K13" s="55"/>
+      <c r="L13" s="52"/>
       <c r="N13" s="8"/>
     </row>
     <row r="14" spans="2:14" ht="20.100000000000001" customHeight="1">
-      <c r="B14" s="49"/>
-      <c r="C14" s="39" t="s">
+      <c r="B14" s="59"/>
+      <c r="C14" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="H14" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="I14" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="J14" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="K14" s="52">
+      <c r="D14" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="H14" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="I14" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="J14" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="K14" s="54">
         <f t="shared" ref="K14" si="2">SUM(D15+E15+F15+G15+H15+I15+J15)</f>
-        <v>34</v>
-      </c>
-      <c r="L14" s="64" t="s">
+        <v>14</v>
+      </c>
+      <c r="L14" s="47" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="15" spans="2:14" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B15" s="49"/>
-      <c r="C15" s="40"/>
-      <c r="D15" s="26">
-        <v>6</v>
-      </c>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26">
-        <v>6</v>
-      </c>
-      <c r="H15" s="26">
-        <v>6</v>
-      </c>
+      <c r="B15" s="59"/>
+      <c r="C15" s="57"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
       <c r="I15" s="26">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J15" s="26">
-        <v>8</v>
-      </c>
-      <c r="K15" s="69"/>
-      <c r="L15" s="65"/>
+        <v>7</v>
+      </c>
+      <c r="K15" s="58"/>
+      <c r="L15" s="48"/>
     </row>
     <row r="16" spans="2:14" ht="47.25" customHeight="1" thickBot="1">
       <c r="B16" s="15"/>
     </row>
     <row r="17" spans="2:12" ht="20.100000000000001" customHeight="1">
-      <c r="B17" s="55" t="s">
+      <c r="B17" s="62" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="5"/>
@@ -1405,14 +1459,14 @@
       <c r="J17" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="K17" s="66" t="s">
+      <c r="K17" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="L17" s="67"/>
+      <c r="L17" s="50"/>
     </row>
     <row r="18" spans="2:12" ht="20.100000000000001" customHeight="1">
-      <c r="B18" s="55"/>
-      <c r="C18" s="50" t="s">
+      <c r="B18" s="62"/>
+      <c r="C18" s="60" t="s">
         <v>9</v>
       </c>
       <c r="D18" s="20"/>
@@ -1422,12 +1476,12 @@
       <c r="H18" s="20"/>
       <c r="I18" s="20"/>
       <c r="J18" s="20"/>
-      <c r="K18" s="41"/>
-      <c r="L18" s="64"/>
+      <c r="K18" s="63"/>
+      <c r="L18" s="47"/>
     </row>
     <row r="19" spans="2:12" ht="20.100000000000001" customHeight="1">
-      <c r="B19" s="55"/>
-      <c r="C19" s="51"/>
+      <c r="B19" s="62"/>
+      <c r="C19" s="61"/>
       <c r="D19" s="24"/>
       <c r="E19" s="24"/>
       <c r="F19" s="24"/>
@@ -1435,12 +1489,12 @@
       <c r="H19" s="24"/>
       <c r="I19" s="24"/>
       <c r="J19" s="24"/>
-      <c r="K19" s="56"/>
-      <c r="L19" s="68"/>
+      <c r="K19" s="64"/>
+      <c r="L19" s="51"/>
     </row>
     <row r="20" spans="2:12" ht="20.100000000000001" customHeight="1">
-      <c r="B20" s="55"/>
-      <c r="C20" s="39" t="s">
+      <c r="B20" s="62"/>
+      <c r="C20" s="56" t="s">
         <v>10</v>
       </c>
       <c r="D20" s="21"/>
@@ -1450,12 +1504,12 @@
       <c r="H20" s="22"/>
       <c r="I20" s="22"/>
       <c r="J20" s="22"/>
-      <c r="K20" s="41"/>
-      <c r="L20" s="54"/>
+      <c r="K20" s="63"/>
+      <c r="L20" s="52"/>
     </row>
     <row r="21" spans="2:12" ht="20.100000000000001" customHeight="1">
-      <c r="B21" s="55"/>
-      <c r="C21" s="57"/>
+      <c r="B21" s="62"/>
+      <c r="C21" s="65"/>
       <c r="D21" s="25"/>
       <c r="E21" s="26"/>
       <c r="F21" s="26"/>
@@ -1463,13 +1517,13 @@
       <c r="H21" s="26"/>
       <c r="I21" s="26"/>
       <c r="J21" s="26"/>
-      <c r="K21" s="56"/>
-      <c r="L21" s="58"/>
+      <c r="K21" s="64"/>
+      <c r="L21" s="53"/>
     </row>
     <row r="22" spans="2:12" ht="20.100000000000001" customHeight="1">
-      <c r="B22" s="55"/>
-      <c r="C22" s="39" t="s">
-        <v>29</v>
+      <c r="B22" s="62"/>
+      <c r="C22" s="56" t="s">
+        <v>27</v>
       </c>
       <c r="D22" s="23"/>
       <c r="E22" s="23"/>
@@ -1478,12 +1532,12 @@
       <c r="H22" s="23"/>
       <c r="I22" s="23"/>
       <c r="J22" s="23"/>
-      <c r="K22" s="41"/>
-      <c r="L22" s="54"/>
+      <c r="K22" s="63"/>
+      <c r="L22" s="52"/>
     </row>
     <row r="23" spans="2:12" ht="20.100000000000001" customHeight="1">
-      <c r="B23" s="55"/>
-      <c r="C23" s="57"/>
+      <c r="B23" s="62"/>
+      <c r="C23" s="65"/>
       <c r="D23" s="26"/>
       <c r="E23" s="26"/>
       <c r="F23" s="26"/>
@@ -1491,12 +1545,12 @@
       <c r="H23" s="26"/>
       <c r="I23" s="26"/>
       <c r="J23" s="26"/>
-      <c r="K23" s="56"/>
-      <c r="L23" s="54"/>
+      <c r="K23" s="64"/>
+      <c r="L23" s="52"/>
     </row>
     <row r="24" spans="2:12" ht="20.100000000000001" customHeight="1">
-      <c r="B24" s="55"/>
-      <c r="C24" s="39" t="s">
+      <c r="B24" s="62"/>
+      <c r="C24" s="56" t="s">
         <v>12</v>
       </c>
       <c r="D24" s="23"/>
@@ -1506,12 +1560,12 @@
       <c r="H24" s="23"/>
       <c r="I24" s="23"/>
       <c r="J24" s="23"/>
-      <c r="K24" s="41"/>
-      <c r="L24" s="64"/>
+      <c r="K24" s="63"/>
+      <c r="L24" s="47"/>
     </row>
     <row r="25" spans="2:12" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B25" s="55"/>
-      <c r="C25" s="40"/>
+      <c r="B25" s="62"/>
+      <c r="C25" s="57"/>
       <c r="D25" s="26"/>
       <c r="E25" s="26"/>
       <c r="F25" s="26"/>
@@ -1519,8 +1573,8 @@
       <c r="H25" s="26"/>
       <c r="I25" s="26"/>
       <c r="J25" s="26"/>
-      <c r="K25" s="42"/>
-      <c r="L25" s="65"/>
+      <c r="K25" s="72"/>
+      <c r="L25" s="48"/>
     </row>
     <row r="30" spans="2:12">
       <c r="E30" s="9" t="s">
@@ -1540,7 +1594,7 @@
       </c>
     </row>
     <row r="31" spans="2:12">
-      <c r="E31" s="61" t="s">
+      <c r="E31" s="41" t="s">
         <v>9</v>
       </c>
       <c r="F31" s="10" t="s">
@@ -1548,18 +1602,18 @@
       </c>
       <c r="G31" s="10">
         <f>K8</f>
-        <v>40</v>
-      </c>
-      <c r="H31" s="45">
+        <v>32</v>
+      </c>
+      <c r="H31" s="43">
         <f>G32-G31</f>
-        <v>-40</v>
-      </c>
-      <c r="I31" s="63">
+        <v>-32</v>
+      </c>
+      <c r="I31" s="45">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="2:12">
-      <c r="E32" s="62"/>
+      <c r="E32" s="42"/>
       <c r="F32" s="11" t="s">
         <v>17</v>
       </c>
@@ -1567,11 +1621,11 @@
         <f>K9</f>
         <v>0</v>
       </c>
-      <c r="H32" s="46"/>
-      <c r="I32" s="47"/>
+      <c r="H32" s="44"/>
+      <c r="I32" s="46"/>
     </row>
     <row r="33" spans="5:9">
-      <c r="E33" s="43" t="s">
+      <c r="E33" s="73" t="s">
         <v>10</v>
       </c>
       <c r="F33" s="11" t="s">
@@ -1581,17 +1635,17 @@
         <f>K10</f>
         <v>40</v>
       </c>
-      <c r="H33" s="45">
+      <c r="H33" s="43">
         <f>G34-G33</f>
         <v>-40</v>
       </c>
-      <c r="I33" s="47">
+      <c r="I33" s="46">
         <f>G34/G33</f>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="5:9">
-      <c r="E34" s="48"/>
+      <c r="E34" s="75"/>
       <c r="F34" s="11" t="s">
         <v>17</v>
       </c>
@@ -1599,11 +1653,11 @@
         <f>K20</f>
         <v>0</v>
       </c>
-      <c r="H34" s="46"/>
-      <c r="I34" s="47"/>
+      <c r="H34" s="44"/>
+      <c r="I34" s="46"/>
     </row>
     <row r="35" spans="5:9">
-      <c r="E35" s="43" t="s">
+      <c r="E35" s="73" t="s">
         <v>11</v>
       </c>
       <c r="F35" s="11" t="s">
@@ -1613,17 +1667,17 @@
         <f>K12</f>
         <v>30</v>
       </c>
-      <c r="H35" s="45">
+      <c r="H35" s="43">
         <f>G36-G35</f>
         <v>-30</v>
       </c>
-      <c r="I35" s="47">
+      <c r="I35" s="46">
         <f>G36/G35</f>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="5:9">
-      <c r="E36" s="48"/>
+      <c r="E36" s="75"/>
       <c r="F36" s="11" t="s">
         <v>17</v>
       </c>
@@ -1631,11 +1685,11 @@
         <f>K22</f>
         <v>0</v>
       </c>
-      <c r="H36" s="46"/>
-      <c r="I36" s="47"/>
+      <c r="H36" s="44"/>
+      <c r="I36" s="46"/>
     </row>
     <row r="37" spans="5:9">
-      <c r="E37" s="43" t="s">
+      <c r="E37" s="73" t="s">
         <v>12</v>
       </c>
       <c r="F37" s="11" t="s">
@@ -1643,19 +1697,19 @@
       </c>
       <c r="G37" s="11">
         <f>K14</f>
-        <v>34</v>
-      </c>
-      <c r="H37" s="45">
+        <v>14</v>
+      </c>
+      <c r="H37" s="43">
         <f>G38-G37</f>
-        <v>-34</v>
-      </c>
-      <c r="I37" s="47">
+        <v>-14</v>
+      </c>
+      <c r="I37" s="46">
         <f>G38/G37</f>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="5:9" ht="15.75" thickBot="1">
-      <c r="E38" s="44"/>
+      <c r="E38" s="74"/>
       <c r="F38" s="11" t="s">
         <v>17</v>
       </c>
@@ -1663,11 +1717,11 @@
         <f>K24</f>
         <v>0</v>
       </c>
-      <c r="H38" s="46"/>
-      <c r="I38" s="47"/>
+      <c r="H38" s="44"/>
+      <c r="I38" s="46"/>
     </row>
     <row r="39" spans="5:9">
-      <c r="E39" s="37" t="s">
+      <c r="E39" s="70" t="s">
         <v>8</v>
       </c>
       <c r="F39" s="16" t="s">
@@ -1675,19 +1729,19 @@
       </c>
       <c r="G39" s="18">
         <f>SUM(K8+K10+K12+K14)</f>
-        <v>144</v>
-      </c>
-      <c r="H39" s="33">
+        <v>116</v>
+      </c>
+      <c r="H39" s="66">
         <f>G40-G39</f>
-        <v>-144</v>
-      </c>
-      <c r="I39" s="35">
+        <v>-116</v>
+      </c>
+      <c r="I39" s="68">
         <f>G40/G39</f>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="5:9" ht="15.75" thickBot="1">
-      <c r="E40" s="38"/>
+      <c r="E40" s="71"/>
       <c r="F40" s="17" t="s">
         <v>23</v>
       </c>
@@ -1695,11 +1749,40 @@
         <f>K18+K20+K22+K24</f>
         <v>0</v>
       </c>
-      <c r="H40" s="34"/>
-      <c r="I40" s="36"/>
+      <c r="H40" s="67"/>
+      <c r="I40" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="45">
+    <mergeCell ref="H39:H40"/>
+    <mergeCell ref="I39:I40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="K24:K25"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="H37:H38"/>
+    <mergeCell ref="I37:I38"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="H33:H34"/>
+    <mergeCell ref="I33:I34"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="H35:H36"/>
+    <mergeCell ref="I35:I36"/>
+    <mergeCell ref="B7:B15"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="B17:B25"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="K20:K21"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="L20:L21"/>
     <mergeCell ref="C3:L3"/>
     <mergeCell ref="C4:L4"/>
     <mergeCell ref="E31:E32"/>
@@ -1716,35 +1799,6 @@
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="K14:K15"/>
     <mergeCell ref="L18:L19"/>
-    <mergeCell ref="B7:B15"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="B17:B25"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="K20:K21"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="L20:L21"/>
-    <mergeCell ref="H39:H40"/>
-    <mergeCell ref="I39:I40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="K24:K25"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="H37:H38"/>
-    <mergeCell ref="I37:I38"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="H33:H34"/>
-    <mergeCell ref="I33:I34"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="H35:H36"/>
-    <mergeCell ref="I35:I36"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.71212121212121215" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -1761,10 +1815,10 @@
   <sheetPr codeName="Feuil2">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B3:N38"/>
+  <dimension ref="B3:P38"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1776,65 +1830,65 @@
     <col min="13" max="13" width="2.7109375" style="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:14" ht="46.5">
-      <c r="C3" s="59" t="s">
+    <row r="3" spans="2:16" ht="46.5">
+      <c r="C3" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="59"/>
-      <c r="J3" s="59"/>
-      <c r="K3" s="59"/>
-      <c r="L3" s="59"/>
-    </row>
-    <row r="4" spans="2:14" ht="22.5" customHeight="1">
-      <c r="C4" s="60" t="str">
-        <f>D6&amp;" JUIN AU "&amp;J6&amp;" JUIN"</f>
-        <v>10 JUIN AU 16 JUIN</v>
-      </c>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="60"/>
-    </row>
-    <row r="5" spans="2:14" ht="36" customHeight="1">
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+    </row>
+    <row r="4" spans="2:16" ht="22.5" customHeight="1">
+      <c r="C4" s="40" t="str">
+        <f>D6&amp;" JUILLET AU "&amp;J6&amp;" JUILLET"</f>
+        <v>22 JUILLET AU 28 JUILLET</v>
+      </c>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
+    </row>
+    <row r="5" spans="2:16" ht="36" customHeight="1">
       <c r="E5" s="1"/>
       <c r="F5" s="2"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="2:14" ht="22.5" customHeight="1" thickBot="1">
+    <row r="6" spans="2:16" ht="22.5" customHeight="1" thickBot="1">
       <c r="D6" s="3">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E6" s="4">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="F6" s="3">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="G6" s="4">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="H6" s="3">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="I6" s="4">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="J6" s="3">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14" ht="20.100000000000001" customHeight="1">
-      <c r="B7" s="49" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" ht="20.100000000000001" customHeight="1">
+      <c r="B7" s="59" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="5"/>
@@ -1859,14 +1913,14 @@
       <c r="J7" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="K7" s="70" t="s">
+      <c r="K7" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="L7" s="67"/>
-    </row>
-    <row r="8" spans="2:14" ht="20.100000000000001" customHeight="1">
-      <c r="B8" s="49"/>
-      <c r="C8" s="50" t="s">
+      <c r="L7" s="50"/>
+    </row>
+    <row r="8" spans="2:16" ht="20.100000000000001" customHeight="1">
+      <c r="B8" s="59"/>
+      <c r="C8" s="60" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="29" t="s">
@@ -1886,17 +1940,17 @@
       </c>
       <c r="I8" s="28"/>
       <c r="J8" s="28"/>
-      <c r="K8" s="52">
+      <c r="K8" s="54">
         <f>SUM(D9+E9+F9+G9+H9+I9+J9)</f>
         <v>40</v>
       </c>
-      <c r="L8" s="64" t="s">
+      <c r="L8" s="47" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="2:14" ht="20.100000000000001" customHeight="1">
-      <c r="B9" s="49"/>
-      <c r="C9" s="51"/>
+    <row r="9" spans="2:16" ht="20.100000000000001" customHeight="1">
+      <c r="B9" s="59"/>
+      <c r="C9" s="61"/>
       <c r="D9" s="27">
         <v>8</v>
       </c>
@@ -1914,95 +1968,78 @@
       </c>
       <c r="I9" s="24"/>
       <c r="J9" s="24"/>
-      <c r="K9" s="53"/>
-      <c r="L9" s="68"/>
-    </row>
-    <row r="10" spans="2:14" ht="20.100000000000001" customHeight="1">
-      <c r="B10" s="49"/>
-      <c r="C10" s="39" t="s">
+      <c r="K9" s="55"/>
+      <c r="L9" s="51"/>
+      <c r="P9">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" ht="20.100000000000001" customHeight="1">
+      <c r="B10" s="59"/>
+      <c r="C10" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="G10" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="H10" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="I10" s="22"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="41">
+      <c r="D10" s="79"/>
+      <c r="E10" s="79"/>
+      <c r="F10" s="79"/>
+      <c r="G10" s="79"/>
+      <c r="H10" s="79"/>
+      <c r="I10" s="80"/>
+      <c r="J10" s="80"/>
+      <c r="K10" s="63">
         <f t="shared" ref="K10" si="0">SUM(D11+E11+F11+G11+H11+I11+J11)</f>
-        <v>40</v>
-      </c>
-      <c r="L10" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="L10" s="52" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="2:14" ht="20.100000000000001" customHeight="1">
-      <c r="B11" s="49"/>
-      <c r="C11" s="57"/>
-      <c r="D11" s="25">
-        <v>8</v>
-      </c>
-      <c r="E11" s="25">
-        <v>8</v>
-      </c>
-      <c r="F11" s="25">
-        <v>8</v>
-      </c>
-      <c r="G11" s="25">
-        <v>8</v>
-      </c>
-      <c r="H11" s="25">
-        <v>8</v>
-      </c>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="56"/>
-      <c r="L11" s="58"/>
-    </row>
-    <row r="12" spans="2:14" ht="20.100000000000001" customHeight="1">
-      <c r="B12" s="49"/>
-      <c r="C12" s="39" t="s">
-        <v>29</v>
+    <row r="11" spans="2:16" ht="20.100000000000001" customHeight="1">
+      <c r="B11" s="59"/>
+      <c r="C11" s="65"/>
+      <c r="D11" s="81"/>
+      <c r="E11" s="81"/>
+      <c r="F11" s="81"/>
+      <c r="G11" s="81"/>
+      <c r="H11" s="81"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="64"/>
+      <c r="L11" s="53"/>
+    </row>
+    <row r="12" spans="2:16" ht="20.100000000000001" customHeight="1">
+      <c r="B12" s="59"/>
+      <c r="C12" s="56" t="s">
+        <v>27</v>
       </c>
       <c r="D12" s="32"/>
       <c r="E12" s="32"/>
       <c r="F12" s="32" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G12" s="32" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H12" s="32" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I12" s="32" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J12" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="K12" s="41">
+        <v>28</v>
+      </c>
+      <c r="K12" s="63">
         <f t="shared" ref="K12" si="1">SUM(D13+E13+F13+G13+H13+I13+J13)</f>
         <v>30</v>
       </c>
-      <c r="L12" s="54" t="s">
+      <c r="L12" s="52" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="2:14" ht="20.100000000000001" customHeight="1">
-      <c r="B13" s="49"/>
-      <c r="C13" s="57"/>
+    <row r="13" spans="2:16" ht="20.100000000000001" customHeight="1">
+      <c r="B13" s="59"/>
+      <c r="C13" s="65"/>
       <c r="D13" s="26"/>
       <c r="E13" s="26"/>
       <c r="F13" s="26">
@@ -2020,68 +2057,68 @@
       <c r="J13" s="26">
         <v>6</v>
       </c>
-      <c r="K13" s="56"/>
-      <c r="L13" s="54"/>
+      <c r="K13" s="64"/>
+      <c r="L13" s="52"/>
       <c r="N13" s="8"/>
     </row>
-    <row r="14" spans="2:14" ht="20.100000000000001" customHeight="1">
-      <c r="B14" s="49"/>
-      <c r="C14" s="39" t="s">
+    <row r="14" spans="2:16" ht="20.100000000000001" customHeight="1">
+      <c r="B14" s="59"/>
+      <c r="C14" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="H14" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="I14" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="J14" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="K14" s="41">
+      <c r="D14" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="36"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="H14" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="I14" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="J14" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="K14" s="63">
         <f>SUM(D15+E15+F15+G15+H15+I15+J15)</f>
-        <v>34</v>
-      </c>
-      <c r="L14" s="64" t="s">
+        <v>35</v>
+      </c>
+      <c r="L14" s="47" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="2:14" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B15" s="49"/>
-      <c r="C15" s="40"/>
-      <c r="D15" s="26">
-        <v>6</v>
-      </c>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26">
-        <v>6</v>
-      </c>
-      <c r="H15" s="26">
-        <v>6</v>
-      </c>
-      <c r="I15" s="26">
-        <v>8</v>
-      </c>
-      <c r="J15" s="26">
-        <v>8</v>
-      </c>
-      <c r="K15" s="42"/>
-      <c r="L15" s="65"/>
-    </row>
-    <row r="16" spans="2:14" ht="47.25" customHeight="1" thickBot="1">
+    <row r="15" spans="2:16" ht="20.100000000000001" customHeight="1" thickBot="1">
+      <c r="B15" s="59"/>
+      <c r="C15" s="57"/>
+      <c r="D15" s="38">
+        <v>7</v>
+      </c>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="38">
+        <v>7</v>
+      </c>
+      <c r="H15" s="38">
+        <v>7</v>
+      </c>
+      <c r="I15" s="38">
+        <v>7</v>
+      </c>
+      <c r="J15" s="38">
+        <v>7</v>
+      </c>
+      <c r="K15" s="72"/>
+      <c r="L15" s="48"/>
+    </row>
+    <row r="16" spans="2:16" ht="47.25" customHeight="1" thickBot="1">
       <c r="B16" s="15"/>
     </row>
     <row r="17" spans="2:12" ht="20.100000000000001" customHeight="1">
-      <c r="B17" s="55" t="s">
+      <c r="B17" s="62" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="5"/>
@@ -2106,14 +2143,14 @@
       <c r="J17" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="K17" s="66" t="s">
+      <c r="K17" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="L17" s="67"/>
+      <c r="L17" s="50"/>
     </row>
     <row r="18" spans="2:12" ht="20.100000000000001" customHeight="1">
-      <c r="B18" s="55"/>
-      <c r="C18" s="50" t="s">
+      <c r="B18" s="62"/>
+      <c r="C18" s="60" t="s">
         <v>9</v>
       </c>
       <c r="D18" s="20"/>
@@ -2123,17 +2160,17 @@
       <c r="H18" s="20"/>
       <c r="I18" s="20"/>
       <c r="J18" s="20"/>
-      <c r="K18" s="41">
+      <c r="K18" s="63">
         <f>SUM(D19+E19+F19+G19+H19+I19+J19)</f>
         <v>0</v>
       </c>
-      <c r="L18" s="64" t="s">
+      <c r="L18" s="47" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="19" spans="2:12" ht="20.100000000000001" customHeight="1">
-      <c r="B19" s="55"/>
-      <c r="C19" s="51"/>
+      <c r="B19" s="62"/>
+      <c r="C19" s="61"/>
       <c r="D19" s="24"/>
       <c r="E19" s="24"/>
       <c r="F19" s="24"/>
@@ -2141,12 +2178,12 @@
       <c r="H19" s="24"/>
       <c r="I19" s="24"/>
       <c r="J19" s="24"/>
-      <c r="K19" s="56"/>
-      <c r="L19" s="68"/>
+      <c r="K19" s="64"/>
+      <c r="L19" s="51"/>
     </row>
     <row r="20" spans="2:12" ht="20.100000000000001" customHeight="1">
-      <c r="B20" s="55"/>
-      <c r="C20" s="39" t="s">
+      <c r="B20" s="62"/>
+      <c r="C20" s="56" t="s">
         <v>10</v>
       </c>
       <c r="D20" s="21"/>
@@ -2156,17 +2193,17 @@
       <c r="H20" s="22"/>
       <c r="I20" s="22"/>
       <c r="J20" s="22"/>
-      <c r="K20" s="41">
+      <c r="K20" s="63">
         <f>SUM(D21+E21+F21+G21+H21+I21+J21)</f>
         <v>0</v>
       </c>
-      <c r="L20" s="54" t="s">
+      <c r="L20" s="52" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="21" spans="2:12" ht="20.100000000000001" customHeight="1">
-      <c r="B21" s="55"/>
-      <c r="C21" s="57"/>
+      <c r="B21" s="62"/>
+      <c r="C21" s="65"/>
       <c r="D21" s="25"/>
       <c r="E21" s="26"/>
       <c r="F21" s="26"/>
@@ -2174,13 +2211,13 @@
       <c r="H21" s="26"/>
       <c r="I21" s="26"/>
       <c r="J21" s="26"/>
-      <c r="K21" s="56"/>
-      <c r="L21" s="58"/>
+      <c r="K21" s="64"/>
+      <c r="L21" s="53"/>
     </row>
     <row r="22" spans="2:12" ht="20.100000000000001" customHeight="1">
-      <c r="B22" s="55"/>
-      <c r="C22" s="39" t="s">
-        <v>29</v>
+      <c r="B22" s="62"/>
+      <c r="C22" s="56" t="s">
+        <v>27</v>
       </c>
       <c r="D22" s="23"/>
       <c r="E22" s="23"/>
@@ -2189,17 +2226,17 @@
       <c r="H22" s="23"/>
       <c r="I22" s="23"/>
       <c r="J22" s="23"/>
-      <c r="K22" s="41">
+      <c r="K22" s="63">
         <f t="shared" ref="K22" si="2">SUM(D23+E23+F23+G23+H23+I23+J23)</f>
         <v>0</v>
       </c>
-      <c r="L22" s="54" t="s">
+      <c r="L22" s="52" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="23" spans="2:12" ht="20.100000000000001" customHeight="1">
-      <c r="B23" s="55"/>
-      <c r="C23" s="57"/>
+      <c r="B23" s="62"/>
+      <c r="C23" s="65"/>
       <c r="D23" s="26"/>
       <c r="E23" s="26"/>
       <c r="F23" s="26"/>
@@ -2207,12 +2244,12 @@
       <c r="H23" s="26"/>
       <c r="I23" s="26"/>
       <c r="J23" s="26"/>
-      <c r="K23" s="56"/>
-      <c r="L23" s="54"/>
+      <c r="K23" s="64"/>
+      <c r="L23" s="52"/>
     </row>
     <row r="24" spans="2:12" ht="20.100000000000001" customHeight="1">
-      <c r="B24" s="55"/>
-      <c r="C24" s="39" t="s">
+      <c r="B24" s="62"/>
+      <c r="C24" s="56" t="s">
         <v>12</v>
       </c>
       <c r="D24" s="23"/>
@@ -2222,17 +2259,17 @@
       <c r="H24" s="23"/>
       <c r="I24" s="23"/>
       <c r="J24" s="23"/>
-      <c r="K24" s="41">
+      <c r="K24" s="63">
         <f t="shared" ref="K24" si="3">SUM(D25+E25+F25+G25+H25+I25+J25)</f>
         <v>0</v>
       </c>
-      <c r="L24" s="64" t="s">
+      <c r="L24" s="47" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="25" spans="2:12" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B25" s="55"/>
-      <c r="C25" s="40"/>
+      <c r="B25" s="62"/>
+      <c r="C25" s="57"/>
       <c r="D25" s="26"/>
       <c r="E25" s="26"/>
       <c r="F25" s="26"/>
@@ -2240,8 +2277,8 @@
       <c r="H25" s="26"/>
       <c r="I25" s="26"/>
       <c r="J25" s="26"/>
-      <c r="K25" s="42"/>
-      <c r="L25" s="65"/>
+      <c r="K25" s="72"/>
+      <c r="L25" s="48"/>
     </row>
     <row r="30" spans="2:12">
       <c r="E30" s="9" t="s">
@@ -2261,7 +2298,7 @@
       </c>
     </row>
     <row r="31" spans="2:12">
-      <c r="E31" s="61" t="s">
+      <c r="E31" s="41" t="s">
         <v>9</v>
       </c>
       <c r="F31" s="10" t="s">
@@ -2271,16 +2308,16 @@
         <f>K8</f>
         <v>40</v>
       </c>
-      <c r="H31" s="45">
+      <c r="H31" s="43">
         <f>G32-G31</f>
         <v>-40</v>
       </c>
-      <c r="I31" s="63">
+      <c r="I31" s="45">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="2:12">
-      <c r="E32" s="62"/>
+      <c r="E32" s="42"/>
       <c r="F32" s="11" t="s">
         <v>17</v>
       </c>
@@ -2288,11 +2325,11 @@
         <f>K18</f>
         <v>0</v>
       </c>
-      <c r="H32" s="46"/>
-      <c r="I32" s="47"/>
+      <c r="H32" s="44"/>
+      <c r="I32" s="46"/>
     </row>
     <row r="33" spans="5:9">
-      <c r="E33" s="43" t="s">
+      <c r="E33" s="73" t="s">
         <v>10</v>
       </c>
       <c r="F33" s="11" t="s">
@@ -2300,19 +2337,19 @@
       </c>
       <c r="G33" s="11">
         <f>K10</f>
-        <v>40</v>
-      </c>
-      <c r="H33" s="45">
+        <v>0</v>
+      </c>
+      <c r="H33" s="43">
         <f>G34-G33</f>
-        <v>-40</v>
-      </c>
-      <c r="I33" s="47">
+        <v>0</v>
+      </c>
+      <c r="I33" s="46" t="e">
         <f>G34/G33</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="34" spans="5:9">
-      <c r="E34" s="48"/>
+      <c r="E34" s="75"/>
       <c r="F34" s="11" t="s">
         <v>17</v>
       </c>
@@ -2320,11 +2357,11 @@
         <f>K20</f>
         <v>0</v>
       </c>
-      <c r="H34" s="46"/>
-      <c r="I34" s="47"/>
+      <c r="H34" s="44"/>
+      <c r="I34" s="46"/>
     </row>
     <row r="35" spans="5:9">
-      <c r="E35" s="43" t="s">
+      <c r="E35" s="73" t="s">
         <v>11</v>
       </c>
       <c r="F35" s="11" t="s">
@@ -2334,17 +2371,17 @@
         <f>K12</f>
         <v>30</v>
       </c>
-      <c r="H35" s="45">
+      <c r="H35" s="43">
         <f>G36-G35</f>
         <v>-30</v>
       </c>
-      <c r="I35" s="47">
+      <c r="I35" s="46">
         <f>G36/G35</f>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="5:9">
-      <c r="E36" s="48"/>
+      <c r="E36" s="75"/>
       <c r="F36" s="11" t="s">
         <v>17</v>
       </c>
@@ -2352,11 +2389,11 @@
         <f>K22</f>
         <v>0</v>
       </c>
-      <c r="H36" s="46"/>
-      <c r="I36" s="47"/>
+      <c r="H36" s="44"/>
+      <c r="I36" s="46"/>
     </row>
     <row r="37" spans="5:9">
-      <c r="E37" s="43" t="s">
+      <c r="E37" s="73" t="s">
         <v>12</v>
       </c>
       <c r="F37" s="11" t="s">
@@ -2364,19 +2401,19 @@
       </c>
       <c r="G37" s="11">
         <f>K14</f>
-        <v>34</v>
-      </c>
-      <c r="H37" s="45">
+        <v>35</v>
+      </c>
+      <c r="H37" s="43">
         <f>G38-G37</f>
-        <v>-34</v>
-      </c>
-      <c r="I37" s="47">
+        <v>-35</v>
+      </c>
+      <c r="I37" s="46">
         <f>G38/G37</f>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="5:9">
-      <c r="E38" s="48"/>
+      <c r="E38" s="75"/>
       <c r="F38" s="12" t="s">
         <v>17</v>
       </c>
@@ -2384,37 +2421,11 @@
         <f>K24</f>
         <v>0</v>
       </c>
-      <c r="H38" s="71"/>
-      <c r="I38" s="72"/>
+      <c r="H38" s="76"/>
+      <c r="I38" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="H31:H32"/>
-    <mergeCell ref="I31:I32"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="H37:H38"/>
-    <mergeCell ref="I37:I38"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="H33:H34"/>
-    <mergeCell ref="I33:I34"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="H35:H36"/>
-    <mergeCell ref="I35:I36"/>
-    <mergeCell ref="B17:B25"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="L18:L19"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="K20:K21"/>
-    <mergeCell ref="L20:L21"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="K24:K25"/>
-    <mergeCell ref="L24:L25"/>
     <mergeCell ref="C3:L3"/>
     <mergeCell ref="C4:L4"/>
     <mergeCell ref="B7:B15"/>
@@ -2431,6 +2442,32 @@
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="K14:K15"/>
     <mergeCell ref="L14:L15"/>
+    <mergeCell ref="B17:B25"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="L18:L19"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="K20:K21"/>
+    <mergeCell ref="L20:L21"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="K24:K25"/>
+    <mergeCell ref="L24:L25"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="I31:I32"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="H37:H38"/>
+    <mergeCell ref="I37:I38"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="H33:H34"/>
+    <mergeCell ref="I33:I34"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="H35:H36"/>
+    <mergeCell ref="I35:I36"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>